<commit_message>
+ barplots to plotting funcs, update figs & readme
</commit_message>
<xml_diff>
--- a/RISA_OUT/Spectra_Metadata.xlsx
+++ b/RISA_OUT/Spectra_Metadata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="87">
   <si>
     <t xml:space="preserve">Time</t>
   </si>
@@ -47,12 +47,6 @@
   </si>
   <si>
     <t xml:space="preserve">cells/mL(measured)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">g/ice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ng/algae</t>
   </si>
   <si>
     <t xml:space="preserve">ppb_calc_frm_cllspermL</t>
@@ -298,7 +292,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -319,6 +313,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -363,13 +362,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -393,10 +400,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P36"/>
+  <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H34" activeCellId="0" sqref="H34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N38" activeCellId="0" sqref="N38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -404,14 +411,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="5.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.64"/>
@@ -463,27 +470,21 @@
       <c r="N1" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="0" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1101</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F2" s="0" t="n">
@@ -499,43 +500,38 @@
         <v>15313</v>
       </c>
       <c r="J2" s="0" t="n">
-        <v>0.45</v>
+        <v>113316.2</v>
       </c>
       <c r="K2" s="0" t="n">
-        <v>5665.81</v>
+        <f aca="false">H2/ (      (((((PI()*4^2)*40)*0.0014)*0.3)/0.917)*10   )</f>
+        <v>10859.0091380408</v>
       </c>
       <c r="L2" s="0" t="n">
-        <v>113316.2</v>
+        <v>0.999</v>
       </c>
       <c r="M2" s="0" t="n">
-        <f aca="false">H2/ ((PI()*4^2*40)*0.0014*0.3*(1/0.917)*10)</f>
-        <v>10859.0091380408</v>
+        <v>6174</v>
       </c>
       <c r="N2" s="0" t="n">
-        <v>0.999</v>
-      </c>
-      <c r="O2" s="0" t="n">
-        <v>6174</v>
-      </c>
-      <c r="P2" s="0" t="n">
-        <f aca="false">ABS(M2-I2)</f>
+        <f aca="false">ABS(K2-I2)</f>
         <v>4453.99086195922</v>
       </c>
+      <c r="S2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>1111</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="F3" s="0" t="n">
@@ -551,44 +547,39 @@
         <v>6688</v>
       </c>
       <c r="J3" s="0" t="n">
-        <v>0.45</v>
+        <v>49491.2</v>
       </c>
       <c r="K3" s="0" t="n">
-        <v>2474.56</v>
+        <f aca="false">H3/ (      (((((PI()*4^2)*40)*0.0014)*0.3)/0.917)*10   )</f>
+        <v>8144.25685353058</v>
       </c>
       <c r="L3" s="0" t="n">
-        <v>49491.2</v>
+        <v>0.997728028739568</v>
       </c>
       <c r="M3" s="0" t="n">
-        <f aca="false">H3/ ((PI()*4^2*40)*0.0014*0.3*(1/0.917)*10)</f>
-        <v>8144.25685353058</v>
+        <f aca="false">1E-034*L3*EXP(87.015*L3)</f>
+        <v>5049.96556216541</v>
       </c>
       <c r="N3" s="0" t="n">
-        <v>0.997728028739568</v>
-      </c>
-      <c r="O3" s="0" t="n">
-        <f aca="false">1E-034*N3*EXP(87.015*N3)</f>
-        <v>5049.96556216556</v>
-      </c>
-      <c r="P3" s="0" t="n">
-        <f aca="false">ABS(M3-I3)</f>
+        <f aca="false">ABS(K3-I3)</f>
         <v>1456.25685353058</v>
       </c>
+      <c r="S3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>1121</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F4" s="0" t="n">
@@ -604,43 +595,39 @@
         <v>57083</v>
       </c>
       <c r="J4" s="0" t="n">
-        <v>0.5</v>
+        <v>422414.2</v>
       </c>
       <c r="K4" s="0" t="n">
-        <v>21120.71</v>
+        <f aca="false">H4/ (      (((((PI()*4^2)*40)*0.0014)*0.3)/0.917)*10   )</f>
+        <v>27147.5228451019</v>
       </c>
       <c r="L4" s="0" t="n">
-        <v>422414.2</v>
+        <v>0.999216423664904</v>
       </c>
       <c r="M4" s="0" t="n">
-        <f aca="false">H4/ ((PI()*4^2*40)*0.0014*0.3*(1/0.917)*10)</f>
-        <v>27147.5228451019</v>
+        <f aca="false">1E-034*L4*EXP(87.015*L4)</f>
+        <v>5756.81736343516</v>
       </c>
       <c r="N4" s="0" t="n">
-        <v>0.999216423664904</v>
-      </c>
-      <c r="O4" s="0" t="n">
-        <f aca="false">1E-034*N4*EXP(87.015*N4)</f>
-        <v>5756.81736343492</v>
-      </c>
-      <c r="P4" s="0" t="n">
-        <f aca="false">ABS(M4-I4)</f>
+        <f aca="false">ABS(K4-I4)</f>
         <v>29935.4771548981</v>
       </c>
+      <c r="S4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>1157</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>21</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="E5" s="1"/>
       <c r="F5" s="0" t="n">
         <v>400</v>
       </c>
@@ -654,44 +641,39 @@
         <v>1313</v>
       </c>
       <c r="J5" s="0" t="n">
-        <v>0.4</v>
+        <v>9716.2</v>
       </c>
       <c r="K5" s="0" t="n">
-        <v>485.81</v>
+        <f aca="false">H5/ (      (((((PI()*4^2)*40)*0.0014)*0.3)/0.917)*10   )</f>
+        <v>5429.50456902039</v>
       </c>
       <c r="L5" s="0" t="n">
-        <v>9716.2</v>
+        <v>1.0003</v>
       </c>
       <c r="M5" s="0" t="n">
-        <f aca="false">H5/ ((PI()*4^2*40)*0.0014*0.3*(1/0.917)*10)</f>
-        <v>5429.50456902039</v>
+        <v>6333</v>
       </c>
       <c r="N5" s="0" t="n">
-        <v>1.0003</v>
-      </c>
-      <c r="O5" s="0" t="n">
-        <v>6333</v>
-      </c>
-      <c r="P5" s="0" t="n">
-        <f aca="false">ABS(M5-I5)</f>
+        <f aca="false">ABS(K5-I5)</f>
         <v>4116.50456902039</v>
       </c>
+      <c r="S5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>1037</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>500</v>
@@ -703,41 +685,36 @@
         <v>50000</v>
       </c>
       <c r="J6" s="0" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="K6" s="0" t="n">
-        <v>0</v>
+        <f aca="false">H6/ (      (((((PI()*4^2)*40)*0.0014)*0.3)/0.917)*10   )</f>
+        <v>5429.50456902039</v>
       </c>
       <c r="L6" s="0" t="n">
-        <v>0</v>
+        <v>0.99927795185688</v>
       </c>
       <c r="M6" s="0" t="n">
-        <f aca="false">H6/ ((PI()*4^2*40)*0.0014*0.3*(1/0.917)*10)</f>
-        <v>5429.50456902039</v>
-      </c>
-      <c r="N6" s="0" t="n">
-        <v>0.99927795185688</v>
-      </c>
-      <c r="O6" s="0" t="n">
-        <f aca="false">1E-034*N6*EXP(87.015*N6)</f>
-        <v>5788.07768897922</v>
-      </c>
+        <f aca="false">1E-034*L6*EXP(87.015*L6)</f>
+        <v>5788.0776889793</v>
+      </c>
+      <c r="S6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>1055</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>29</v>
+      <c r="E7" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>750</v>
@@ -749,41 +726,36 @@
         <v>20000</v>
       </c>
       <c r="J7" s="0" t="n">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="K7" s="0" t="n">
-        <v>0</v>
+        <f aca="false">H7/ (      (((((PI()*4^2)*40)*0.0014)*0.3)/0.917)*10   )</f>
+        <v>2171.80182760816</v>
       </c>
       <c r="L7" s="0" t="n">
-        <v>0</v>
+        <v>0.999262334554645</v>
       </c>
       <c r="M7" s="0" t="n">
-        <f aca="false">H7/ ((PI()*4^2*40)*0.0014*0.3*(1/0.917)*10)</f>
-        <v>2171.80182760816</v>
-      </c>
-      <c r="N7" s="0" t="n">
-        <v>0.999262334554645</v>
-      </c>
-      <c r="O7" s="0" t="n">
-        <f aca="false">1E-034*N7*EXP(87.015*N7)</f>
-        <v>5780.12704668693</v>
-      </c>
+        <f aca="false">1E-034*L7*EXP(87.015*L7)</f>
+        <v>5780.12704668684</v>
+      </c>
+      <c r="S7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>1152</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>400</v>
@@ -798,44 +770,39 @@
         <v>3063</v>
       </c>
       <c r="J8" s="0" t="n">
-        <v>0.4</v>
+        <v>22666.2</v>
       </c>
       <c r="K8" s="0" t="n">
-        <v>1133.31</v>
+        <f aca="false">H8/ (      (((((PI()*4^2)*40)*0.0014)*0.3)/0.917)*10   )</f>
+        <v>8144.25685353058</v>
       </c>
       <c r="L8" s="0" t="n">
-        <v>22666.2</v>
+        <v>0.998803629079593</v>
       </c>
       <c r="M8" s="0" t="n">
-        <f aca="false">H8/ ((PI()*4^2*40)*0.0014*0.3*(1/0.917)*10)</f>
-        <v>8144.25685353058</v>
+        <f aca="false">1E-034*L8*EXP(87.015*L8)</f>
+        <v>5551.41170368124</v>
       </c>
       <c r="N8" s="0" t="n">
-        <v>0.998803629079593</v>
-      </c>
-      <c r="O8" s="0" t="n">
-        <f aca="false">1E-034*N8*EXP(87.015*N8)</f>
-        <v>5551.4117036814</v>
-      </c>
-      <c r="P8" s="0" t="n">
-        <f aca="false">ABS(M8-I8)</f>
+        <f aca="false">ABS(K8-I8)</f>
         <v>5081.25685353058</v>
       </c>
+      <c r="S8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>1302</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="E9" s="1" t="n">
         <v>2</v>
       </c>
       <c r="F9" s="0" t="n">
@@ -851,45 +818,40 @@
         <v>12438</v>
       </c>
       <c r="J9" s="0" t="n">
-        <v>0.4</v>
+        <v>92041.2</v>
       </c>
       <c r="K9" s="0" t="n">
-        <v>4602.06</v>
+        <f aca="false">H9/ (      (((((PI()*4^2)*40)*0.0014)*0.3)/0.917)*10   )</f>
+        <v>16288.5137070612</v>
       </c>
       <c r="L9" s="0" t="n">
-        <v>92041.2</v>
+        <v>1.00112869911369</v>
       </c>
       <c r="M9" s="0" t="n">
-        <f aca="false">H9/ ((PI()*4^2*40)*0.0014*0.3*(1/0.917)*10)</f>
-        <v>16288.5137070612</v>
+        <f aca="false">1E-034*L9*EXP(87.015*L9)</f>
+        <v>6812.05185592986</v>
       </c>
       <c r="N9" s="0" t="n">
-        <v>1.00112869911369</v>
-      </c>
-      <c r="O9" s="0" t="n">
-        <f aca="false">1E-034*N9*EXP(87.015*N9)</f>
-        <v>6812.05185593202</v>
-      </c>
-      <c r="P9" s="0" t="n">
-        <f aca="false">ABS(M9-I9)</f>
+        <f aca="false">ABS(K9-I9)</f>
         <v>3850.51370706116</v>
       </c>
+      <c r="S9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>1134</v>
       </c>
       <c r="B10" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>450</v>
@@ -901,39 +863,35 @@
         <v>100000</v>
       </c>
       <c r="J10" s="0" t="n">
-        <v>0.45</v>
+        <v>0</v>
       </c>
       <c r="K10" s="0" t="n">
-        <v>0</v>
+        <f aca="false">H10/ (      (((((PI()*4^2)*40)*0.0014)*0.3)/0.917)*10   )</f>
+        <v>10859.0091380408</v>
       </c>
       <c r="L10" s="0" t="n">
-        <v>0</v>
+        <v>0.999930747488734</v>
       </c>
       <c r="M10" s="0" t="n">
-        <f aca="false">H10/ ((PI()*4^2*40)*0.0014*0.3*(1/0.917)*10)</f>
-        <v>10859.0091380408</v>
-      </c>
-      <c r="N10" s="0" t="n">
-        <v>0.999930747488734</v>
-      </c>
-      <c r="O10" s="0" t="n">
-        <f aca="false">1E-034*N10*EXP(87.015*N10)</f>
+        <f aca="false">1E-034*L10*EXP(87.015*L10)</f>
         <v>6130.37729530327</v>
       </c>
+      <c r="S10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>1333</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>18</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="E11" s="1"/>
       <c r="F11" s="0" t="n">
         <v>500</v>
       </c>
@@ -947,45 +905,40 @@
         <v>7250</v>
       </c>
       <c r="J11" s="0" t="n">
-        <v>0.5</v>
+        <v>53650</v>
       </c>
       <c r="K11" s="0" t="n">
-        <v>2682.5</v>
+        <f aca="false">H11/ (      (((((PI()*4^2)*40)*0.0014)*0.3)/0.917)*10   )</f>
+        <v>8144.25685353058</v>
       </c>
       <c r="L11" s="0" t="n">
-        <v>53650</v>
+        <v>0.999337107150623</v>
       </c>
       <c r="M11" s="0" t="n">
-        <f aca="false">H11/ ((PI()*4^2*40)*0.0014*0.3*(1/0.917)*10)</f>
-        <v>8144.25685353058</v>
+        <f aca="false">1E-034*L11*EXP(87.015*L11)</f>
+        <v>5818.29245027645</v>
       </c>
       <c r="N11" s="0" t="n">
-        <v>0.999337107150623</v>
-      </c>
-      <c r="O11" s="0" t="n">
-        <f aca="false">1E-034*N11*EXP(87.015*N11)</f>
-        <v>5818.29245027628</v>
-      </c>
-      <c r="P11" s="0" t="n">
-        <f aca="false">ABS(M11-I11)</f>
+        <f aca="false">ABS(K11-I11)</f>
         <v>894.256853530582</v>
       </c>
+      <c r="S11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>1117</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>40</v>
+        <v>22</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>550</v>
@@ -1000,43 +953,39 @@
         <v>44861</v>
       </c>
       <c r="J12" s="0" t="n">
-        <v>0.55</v>
+        <v>331971.4</v>
       </c>
       <c r="K12" s="0" t="n">
-        <v>16598.57</v>
+        <f aca="false">H12/ (      (((((PI()*4^2)*40)*0.0014)*0.3)/0.917)*10   )</f>
+        <v>27147.5228451019</v>
       </c>
       <c r="L12" s="0" t="n">
-        <v>331971.4</v>
+        <v>0.999667713536561</v>
       </c>
       <c r="M12" s="0" t="n">
-        <f aca="false">H12/ ((PI()*4^2*40)*0.0014*0.3*(1/0.917)*10)</f>
-        <v>27147.5228451019</v>
+        <f aca="false">1E-034*L12*EXP(87.015*L12)</f>
+        <v>5990.08325435459</v>
       </c>
       <c r="N12" s="0" t="n">
-        <v>0.999667713536561</v>
-      </c>
-      <c r="O12" s="0" t="n">
-        <f aca="false">1E-034*N12*EXP(87.015*N12)</f>
-        <v>5990.08325435433</v>
-      </c>
-      <c r="P12" s="0" t="n">
-        <f aca="false">ABS(M12-I12)</f>
+        <f aca="false">ABS(K12-I12)</f>
         <v>17713.4771548981</v>
       </c>
+      <c r="S12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>1244</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>24</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E13" s="1"/>
       <c r="F13" s="0" t="n">
         <v>850</v>
       </c>
@@ -1050,44 +999,39 @@
         <v>33229</v>
       </c>
       <c r="J13" s="0" t="n">
-        <v>0.85</v>
+        <v>245894.6</v>
       </c>
       <c r="K13" s="0" t="n">
-        <v>12294.73</v>
+        <f aca="false">H13/ (      (((((PI()*4^2)*40)*0.0014)*0.3)/0.917)*10   )</f>
+        <v>21718.0182760816</v>
       </c>
       <c r="L13" s="0" t="n">
-        <v>245894.6</v>
+        <v>0.999394804902704</v>
       </c>
       <c r="M13" s="0" t="n">
-        <f aca="false">H13/ ((PI()*4^2*40)*0.0014*0.3*(1/0.917)*10)</f>
-        <v>21718.0182760816</v>
+        <f aca="false">1E-034*L13*EXP(87.015*L13)</f>
+        <v>5847.91466122565</v>
       </c>
       <c r="N13" s="0" t="n">
-        <v>0.999394804902704</v>
-      </c>
-      <c r="O13" s="0" t="n">
-        <f aca="false">1E-034*N13*EXP(87.015*N13)</f>
-        <v>5847.91466122582</v>
-      </c>
-      <c r="P13" s="0" t="n">
-        <f aca="false">ABS(M13-I13)</f>
+        <f aca="false">ABS(K13-I13)</f>
         <v>11510.9817239184</v>
       </c>
+      <c r="S13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>1305</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="E14" s="1" t="n">
         <v>3</v>
       </c>
       <c r="F14" s="0" t="n">
@@ -1103,44 +1047,39 @@
         <v>313</v>
       </c>
       <c r="J14" s="0" t="n">
-        <v>0.75</v>
+        <v>2316.2</v>
       </c>
       <c r="K14" s="0" t="n">
-        <v>115.81</v>
+        <f aca="false">H14/ (      (((((PI()*4^2)*40)*0.0014)*0.3)/0.917)*10   )</f>
+        <v>2171.80182760816</v>
       </c>
       <c r="L14" s="0" t="n">
-        <v>2316.2</v>
+        <v>0.998352729027748</v>
       </c>
       <c r="M14" s="0" t="n">
-        <f aca="false">H14/ ((PI()*4^2*40)*0.0014*0.3*(1/0.917)*10)</f>
-        <v>2171.80182760816</v>
+        <f aca="false">1E-034*L14*EXP(87.015*L14)</f>
+        <v>5335.40953886072</v>
       </c>
       <c r="N14" s="0" t="n">
-        <v>0.998352729027748</v>
-      </c>
-      <c r="O14" s="0" t="n">
-        <f aca="false">1E-034*N14*EXP(87.015*N14)</f>
-        <v>5335.40953886087</v>
-      </c>
-      <c r="P14" s="0" t="n">
-        <f aca="false">ABS(M14-I14)</f>
+        <f aca="false">ABS(K14-I14)</f>
         <v>1858.80182760816</v>
       </c>
+      <c r="S14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>1230</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="E15" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F15" s="0" t="n">
@@ -1156,43 +1095,39 @@
         <v>28563</v>
       </c>
       <c r="J15" s="0" t="n">
-        <v>0.4</v>
+        <v>211366.2</v>
       </c>
       <c r="K15" s="0" t="n">
-        <v>10568.31</v>
+        <f aca="false">H15/ (      (((((PI()*4^2)*40)*0.0014)*0.3)/0.917)*10   )</f>
+        <v>27147.5228451019</v>
       </c>
       <c r="L15" s="0" t="n">
-        <v>211366.2</v>
+        <v>1.00096376999254</v>
       </c>
       <c r="M15" s="0" t="n">
-        <f aca="false">H15/ ((PI()*4^2*40)*0.0014*0.3*(1/0.917)*10)</f>
-        <v>27147.5228451019</v>
+        <f aca="false">1E-034*L15*EXP(87.015*L15)</f>
+        <v>6713.88191807834</v>
       </c>
       <c r="N15" s="0" t="n">
-        <v>1.00096376999254</v>
-      </c>
-      <c r="O15" s="0" t="n">
-        <f aca="false">1E-034*N15*EXP(87.015*N15)</f>
-        <v>6713.8819180794</v>
-      </c>
-      <c r="P15" s="0" t="n">
-        <f aca="false">ABS(M15-I15)</f>
+        <f aca="false">ABS(K15-I15)</f>
         <v>1415.47715489806</v>
       </c>
+      <c r="S15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>1132</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>24</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E16" s="1"/>
       <c r="F16" s="0" t="n">
         <v>400</v>
       </c>
@@ -1206,44 +1141,39 @@
         <v>22813</v>
       </c>
       <c r="J16" s="0" t="n">
-        <v>0.4</v>
+        <v>168816.2</v>
       </c>
       <c r="K16" s="0" t="n">
-        <v>8440.81</v>
+        <f aca="false">H16/ (      (((((PI()*4^2)*40)*0.0014)*0.3)/0.917)*10   )</f>
+        <v>27147.5228451019</v>
       </c>
       <c r="L16" s="0" t="n">
-        <v>168816.2</v>
+        <v>0.998899201733255</v>
       </c>
       <c r="M16" s="0" t="n">
-        <f aca="false">H16/ ((PI()*4^2*40)*0.0014*0.3*(1/0.917)*10)</f>
-        <v>27147.5228451019</v>
+        <f aca="false">1E-034*L16*EXP(87.015*L16)</f>
+        <v>5598.30679199573</v>
       </c>
       <c r="N16" s="0" t="n">
-        <v>0.998899201733255</v>
-      </c>
-      <c r="O16" s="0" t="n">
-        <f aca="false">1E-034*N16*EXP(87.015*N16)</f>
-        <v>5598.30679199597</v>
-      </c>
-      <c r="P16" s="0" t="n">
-        <f aca="false">ABS(M16-I16)</f>
+        <f aca="false">ABS(K16-I16)</f>
         <v>4334.52284510194</v>
       </c>
+      <c r="S16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>1143</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="E17" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F17" s="0" t="n">
@@ -1256,40 +1186,35 @@
         <v>75000</v>
       </c>
       <c r="J17" s="0" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="K17" s="0" t="n">
-        <v>0</v>
+        <f aca="false">H17/ (      (((((PI()*4^2)*40)*0.0014)*0.3)/0.917)*10   )</f>
+        <v>8144.25685353058</v>
       </c>
       <c r="L17" s="0" t="n">
-        <v>0</v>
+        <v>0.999400676271843</v>
       </c>
       <c r="M17" s="0" t="n">
-        <f aca="false">H17/ ((PI()*4^2*40)*0.0014*0.3*(1/0.917)*10)</f>
-        <v>8144.25685353058</v>
-      </c>
-      <c r="N17" s="0" t="n">
-        <v>0.999400676271843</v>
-      </c>
-      <c r="O17" s="0" t="n">
-        <f aca="false">1E-034*N17*EXP(87.015*N17)</f>
-        <v>5850.93748131194</v>
-      </c>
+        <f aca="false">1E-034*L17*EXP(87.015*L17)</f>
+        <v>5850.93748131203</v>
+      </c>
+      <c r="S17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>1235</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="E18" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F18" s="0" t="n">
@@ -1302,41 +1227,36 @@
         <v>150000</v>
       </c>
       <c r="J18" s="0" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="K18" s="0" t="n">
-        <v>0</v>
+        <f aca="false">H18/ (      (((((PI()*4^2)*40)*0.0014)*0.3)/0.917)*10   )</f>
+        <v>16288.5137070612</v>
       </c>
       <c r="L18" s="0" t="n">
-        <v>0</v>
+        <v>0.997791919799729</v>
       </c>
       <c r="M18" s="0" t="n">
-        <f aca="false">H18/ ((PI()*4^2*40)*0.0014*0.3*(1/0.917)*10)</f>
-        <v>16288.5137070612</v>
-      </c>
-      <c r="N18" s="0" t="n">
-        <v>0.997791919799729</v>
-      </c>
-      <c r="O18" s="0" t="n">
-        <f aca="false">1E-034*N18*EXP(87.015*N18)</f>
+        <f aca="false">1E-034*L18*EXP(87.015*L18)</f>
         <v>5078.44411950204</v>
       </c>
+      <c r="S18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>1055</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>750</v>
@@ -1348,40 +1268,35 @@
         <v>20000</v>
       </c>
       <c r="J19" s="0" t="n">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="K19" s="0" t="n">
-        <v>0</v>
+        <f aca="false">H19/ (      (((((PI()*4^2)*40)*0.0014)*0.3)/0.917)*10   )</f>
+        <v>2171.80182760816</v>
       </c>
       <c r="L19" s="0" t="n">
-        <v>0</v>
+        <v>0.999262334554645</v>
       </c>
       <c r="M19" s="0" t="n">
-        <f aca="false">H19/ ((PI()*4^2*40)*0.0014*0.3*(1/0.917)*10)</f>
-        <v>2171.80182760816</v>
-      </c>
-      <c r="N19" s="0" t="n">
-        <v>0.999262334554645</v>
-      </c>
-      <c r="O19" s="0" t="n">
-        <f aca="false">1E-034*N19*EXP(87.015*N19)</f>
-        <v>5780.12704668693</v>
-      </c>
+        <f aca="false">1E-034*L19*EXP(87.015*L19)</f>
+        <v>5780.12704668684</v>
+      </c>
+      <c r="S19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>1108</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E20" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="E20" s="1" t="n">
         <v>10</v>
       </c>
       <c r="F20" s="0" t="n">
@@ -1394,41 +1309,36 @@
         <v>250000</v>
       </c>
       <c r="J20" s="0" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="K20" s="0" t="n">
-        <v>0</v>
+        <f aca="false">H20/ (      (((((PI()*4^2)*40)*0.0014)*0.3)/0.917)*10   )</f>
+        <v>27147.5228451019</v>
       </c>
       <c r="L20" s="0" t="n">
-        <v>0</v>
+        <v>1.00180364473015</v>
       </c>
       <c r="M20" s="0" t="n">
-        <f aca="false">H20/ ((PI()*4^2*40)*0.0014*0.3*(1/0.917)*10)</f>
-        <v>27147.5228451019</v>
-      </c>
-      <c r="N20" s="0" t="n">
-        <v>1.00180364473015</v>
-      </c>
-      <c r="O20" s="0" t="n">
-        <f aca="false">1E-034*N20*EXP(87.015*N20)</f>
-        <v>7228.97839625261</v>
-      </c>
+        <f aca="false">1E-034*L20*EXP(87.015*L20)</f>
+        <v>7228.9783962549</v>
+      </c>
+      <c r="S20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>1007</v>
       </c>
       <c r="B21" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>450</v>
@@ -1440,40 +1350,35 @@
         <v>100000</v>
       </c>
       <c r="J21" s="0" t="n">
-        <v>0.45</v>
+        <v>0</v>
       </c>
       <c r="K21" s="0" t="n">
-        <v>0</v>
+        <f aca="false">H21/ (      (((((PI()*4^2)*40)*0.0014)*0.3)/0.917)*10   )</f>
+        <v>10859.0091380408</v>
       </c>
       <c r="L21" s="0" t="n">
-        <v>0</v>
+        <v>1.00005768918511</v>
       </c>
       <c r="M21" s="0" t="n">
-        <f aca="false">H21/ ((PI()*4^2*40)*0.0014*0.3*(1/0.917)*10)</f>
-        <v>10859.0091380408</v>
-      </c>
-      <c r="N21" s="0" t="n">
-        <v>1.00005768918511</v>
-      </c>
-      <c r="O21" s="0" t="n">
-        <f aca="false">1E-034*N21*EXP(87.015*N21)</f>
-        <v>6199.25467542321</v>
-      </c>
+        <f aca="false">1E-034*L21*EXP(87.015*L21)</f>
+        <v>6199.25467542588</v>
+      </c>
+      <c r="S21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>1220</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E22" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="E22" s="1" t="n">
         <v>5</v>
       </c>
       <c r="F22" s="0" t="n">
@@ -1486,40 +1391,35 @@
         <v>250000</v>
       </c>
       <c r="J22" s="0" t="n">
-        <v>0.85</v>
+        <v>0</v>
       </c>
       <c r="K22" s="0" t="n">
-        <v>0</v>
+        <f aca="false">H22/ (      (((((PI()*4^2)*40)*0.0014)*0.3)/0.917)*10   )</f>
+        <v>27147.5228451019</v>
       </c>
       <c r="L22" s="0" t="n">
-        <v>0</v>
+        <v>0.999456975476871</v>
       </c>
       <c r="M22" s="0" t="n">
-        <f aca="false">H22/ ((PI()*4^2*40)*0.0014*0.3*(1/0.917)*10)</f>
-        <v>27147.5228451019</v>
-      </c>
-      <c r="N22" s="0" t="n">
-        <v>0.999456975476871</v>
-      </c>
-      <c r="O22" s="0" t="n">
-        <f aca="false">1E-034*N22*EXP(87.015*N22)</f>
-        <v>5880.00203692252</v>
-      </c>
+        <f aca="false">1E-034*L22*EXP(87.015*L22)</f>
+        <v>5880.00203692269</v>
+      </c>
+      <c r="S22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>1233</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="E23" s="1" t="n">
         <v>5</v>
       </c>
       <c r="F23" s="0" t="n">
@@ -1535,44 +1435,39 @@
         <v>41000</v>
       </c>
       <c r="J23" s="0" t="n">
-        <v>0.75</v>
+        <v>303400</v>
       </c>
       <c r="K23" s="0" t="n">
-        <v>15170</v>
+        <f aca="false">H23/ (      (((((PI()*4^2)*40)*0.0014)*0.3)/0.917)*10   )</f>
+        <v>27147.5228451019</v>
       </c>
       <c r="L23" s="0" t="n">
-        <v>303400</v>
+        <v>1.00180364473015</v>
       </c>
       <c r="M23" s="0" t="n">
-        <f aca="false">H23/ ((PI()*4^2*40)*0.0014*0.3*(1/0.917)*10)</f>
-        <v>27147.5228451019</v>
+        <f aca="false">1E-034*L23*EXP(87.015*L23)</f>
+        <v>7228.9783962549</v>
       </c>
       <c r="N23" s="0" t="n">
-        <v>1.00180364473015</v>
-      </c>
-      <c r="O23" s="0" t="n">
-        <f aca="false">1E-034*N23*EXP(87.015*N23)</f>
-        <v>7228.97839625261</v>
-      </c>
-      <c r="P23" s="0" t="n">
-        <f aca="false">ABS(M23-I23)</f>
+        <f aca="false">ABS(K23-I23)</f>
         <v>13852.4771548981</v>
       </c>
+      <c r="S23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>1247</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E24" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="E24" s="1" t="n">
         <v>2</v>
       </c>
       <c r="F24" s="0" t="n">
@@ -1588,40 +1483,35 @@
         <v>0</v>
       </c>
       <c r="J24" s="0" t="n">
-        <v>0.85</v>
+        <v>0</v>
       </c>
       <c r="K24" s="0" t="n">
-        <v>0</v>
+        <f aca="false">H24/ (      (((((PI()*4^2)*40)*0.0014)*0.3)/0.917)*10   )</f>
+        <v>2171.80182760816</v>
       </c>
       <c r="L24" s="0" t="n">
-        <v>0</v>
+        <v>0.999596077624139</v>
       </c>
       <c r="M24" s="0" t="n">
-        <f aca="false">H24/ ((PI()*4^2*40)*0.0014*0.3*(1/0.917)*10)</f>
-        <v>2171.80182760816</v>
-      </c>
-      <c r="N24" s="0" t="n">
-        <v>0.999596077624139</v>
-      </c>
-      <c r="O24" s="0" t="n">
-        <f aca="false">1E-034*N24*EXP(87.015*N24)</f>
-        <v>5952.434227211</v>
-      </c>
+        <f aca="false">1E-034*L24*EXP(87.015*L24)</f>
+        <v>5952.43422721108</v>
+      </c>
+      <c r="S24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>1200</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E25" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="E25" s="1" t="n">
         <v>2</v>
       </c>
       <c r="F25" s="0" t="n">
@@ -1634,40 +1524,35 @@
         <v>20000</v>
       </c>
       <c r="J25" s="0" t="n">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="K25" s="0" t="n">
-        <v>0</v>
+        <f aca="false">H25/ (      (((((PI()*4^2)*40)*0.0014)*0.3)/0.917)*10   )</f>
+        <v>2171.80182760816</v>
       </c>
       <c r="L25" s="0" t="n">
-        <v>0</v>
+        <v>0.999743346860701</v>
       </c>
       <c r="M25" s="0" t="n">
-        <f aca="false">H25/ ((PI()*4^2*40)*0.0014*0.3*(1/0.917)*10)</f>
-        <v>2171.80182760816</v>
-      </c>
-      <c r="N25" s="0" t="n">
-        <v>0.999743346860701</v>
-      </c>
-      <c r="O25" s="0" t="n">
-        <f aca="false">1E-034*N25*EXP(87.015*N25)</f>
-        <v>6030.09159328888</v>
-      </c>
+        <f aca="false">1E-034*L25*EXP(87.015*L25)</f>
+        <v>6030.09159328879</v>
+      </c>
+      <c r="S25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>1358</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E26" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="E26" s="1" t="n">
         <v>3</v>
       </c>
       <c r="F26" s="0" t="n">
@@ -1683,43 +1568,39 @@
         <v>938</v>
       </c>
       <c r="J26" s="0" t="n">
-        <v>0.9</v>
+        <v>6941.2</v>
       </c>
       <c r="K26" s="0" t="n">
-        <v>347.06</v>
+        <f aca="false">H26/ (      (((((PI()*4^2)*40)*0.0014)*0.3)/0.917)*10   )</f>
+        <v>2171.80182760816</v>
       </c>
       <c r="L26" s="0" t="n">
-        <v>6941.2</v>
+        <v>0.997493061731166</v>
       </c>
       <c r="M26" s="0" t="n">
-        <f aca="false">H26/ ((PI()*4^2*40)*0.0014*0.3*(1/0.917)*10)</f>
-        <v>2171.80182760816</v>
+        <f aca="false">1E-034*L26*EXP(87.015*L26)</f>
+        <v>4946.59885222112</v>
       </c>
       <c r="N26" s="0" t="n">
-        <v>0.997493061731166</v>
-      </c>
-      <c r="O26" s="0" t="n">
-        <f aca="false">1E-034*N26*EXP(87.015*N26)</f>
-        <v>4946.5988522209</v>
-      </c>
-      <c r="P26" s="0" t="n">
-        <f aca="false">ABS(M26-I26)</f>
+        <f aca="false">ABS(K26-I26)</f>
         <v>1233.80182760816</v>
       </c>
+      <c r="S26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>1104</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>24</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E27" s="1"/>
       <c r="F27" s="0" t="n">
         <v>900</v>
       </c>
@@ -1730,39 +1611,35 @@
         <v>250000</v>
       </c>
       <c r="J27" s="0" t="n">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="K27" s="0" t="n">
-        <v>0</v>
+        <f aca="false">H27/ (      (((((PI()*4^2)*40)*0.0014)*0.3)/0.917)*10   )</f>
+        <v>27147.5228451019</v>
       </c>
       <c r="L27" s="0" t="n">
-        <v>0</v>
+        <v>0.998090066749557</v>
       </c>
       <c r="M27" s="0" t="n">
-        <f aca="false">H27/ ((PI()*4^2*40)*0.0014*0.3*(1/0.917)*10)</f>
-        <v>27147.5228451019</v>
-      </c>
-      <c r="N27" s="0" t="n">
-        <v>0.998090066749557</v>
-      </c>
-      <c r="O27" s="0" t="n">
-        <f aca="false">1E-034*N27*EXP(87.015*N27)</f>
-        <v>5213.47676184949</v>
-      </c>
+        <f aca="false">1E-034*L27*EXP(87.015*L27)</f>
+        <v>5213.47676184964</v>
+      </c>
+      <c r="S27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>1046</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>18</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="E28" s="1"/>
       <c r="F28" s="0" t="n">
         <v>400</v>
       </c>
@@ -1773,39 +1650,35 @@
         <v>125000</v>
       </c>
       <c r="J28" s="0" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="K28" s="0" t="n">
-        <v>0</v>
+        <f aca="false">H28/ (      (((((PI()*4^2)*40)*0.0014)*0.3)/0.917)*10   )</f>
+        <v>13573.761422551</v>
       </c>
       <c r="L28" s="0" t="n">
-        <v>0</v>
+        <v>0.998859719334347</v>
       </c>
       <c r="M28" s="0" t="n">
-        <f aca="false">H28/ ((PI()*4^2*40)*0.0014*0.3*(1/0.917)*10)</f>
-        <v>13573.761422551</v>
-      </c>
-      <c r="N28" s="0" t="n">
-        <v>0.998859719334347</v>
-      </c>
-      <c r="O28" s="0" t="n">
-        <f aca="false">1E-034*N28*EXP(87.015*N28)</f>
-        <v>5578.88594941689</v>
-      </c>
+        <f aca="false">1E-034*L28*EXP(87.015*L28)</f>
+        <v>5578.88594941681</v>
+      </c>
+      <c r="S28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <v>1310</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>24</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E29" s="1"/>
       <c r="F29" s="0" t="n">
         <v>400</v>
       </c>
@@ -1816,40 +1689,35 @@
         <v>250000</v>
       </c>
       <c r="J29" s="0" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="K29" s="0" t="n">
-        <v>0</v>
+        <f aca="false">H29/ (      (((((PI()*4^2)*40)*0.0014)*0.3)/0.917)*10   )</f>
+        <v>27147.5228451019</v>
       </c>
       <c r="L29" s="0" t="n">
-        <v>0</v>
+        <v>0.999171594116956</v>
       </c>
       <c r="M29" s="0" t="n">
-        <f aca="false">H29/ ((PI()*4^2*40)*0.0014*0.3*(1/0.917)*10)</f>
-        <v>27147.5228451019</v>
-      </c>
-      <c r="N29" s="0" t="n">
-        <v>0.999171594116956</v>
-      </c>
-      <c r="O29" s="0" t="n">
-        <f aca="false">1E-034*N29*EXP(87.015*N29)</f>
+        <f aca="false">1E-034*L29*EXP(87.015*L29)</f>
         <v>5734.14739233022</v>
       </c>
+      <c r="S29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>1209</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E30" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="E30" s="1" t="n">
         <v>3</v>
       </c>
       <c r="F30" s="0" t="n">
@@ -1865,44 +1733,39 @@
         <v>21125</v>
       </c>
       <c r="J30" s="0" t="n">
-        <v>0.55</v>
+        <v>156325</v>
       </c>
       <c r="K30" s="0" t="n">
-        <v>7816.25</v>
+        <f aca="false">H30/ (      (((((PI()*4^2)*40)*0.0014)*0.3)/0.917)*10   )</f>
+        <v>27147.5228451019</v>
       </c>
       <c r="L30" s="0" t="n">
-        <v>156325</v>
+        <v>0.997172132666332</v>
       </c>
       <c r="M30" s="0" t="n">
-        <f aca="false">H30/ ((PI()*4^2*40)*0.0014*0.3*(1/0.917)*10)</f>
-        <v>27147.5228451019</v>
+        <f aca="false">1E-034*L30*EXP(87.015*L30)</f>
+        <v>4808.82518439531</v>
       </c>
       <c r="N30" s="0" t="n">
-        <v>0.997172132666332</v>
-      </c>
-      <c r="O30" s="0" t="n">
-        <f aca="false">1E-034*N30*EXP(87.015*N30)</f>
-        <v>4808.82518439545</v>
-      </c>
-      <c r="P30" s="0" t="n">
-        <f aca="false">ABS(M30-I30)</f>
+        <f aca="false">ABS(K30-I30)</f>
         <v>6022.52284510194</v>
       </c>
+      <c r="S30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>1159</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E31" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="E31" s="1" t="n">
         <v>2</v>
       </c>
       <c r="F31" s="0" t="n">
@@ -1918,43 +1781,39 @@
         <v>938</v>
       </c>
       <c r="J31" s="0" t="n">
-        <v>0.9</v>
+        <v>6941.2</v>
       </c>
       <c r="K31" s="0" t="n">
-        <v>347.06</v>
+        <f aca="false">H31/ (      (((((PI()*4^2)*40)*0.0014)*0.3)/0.917)*10   )</f>
+        <v>2171.80182760816</v>
       </c>
       <c r="L31" s="0" t="n">
-        <v>6941.2</v>
+        <v>0.997820679177718</v>
       </c>
       <c r="M31" s="0" t="n">
-        <f aca="false">H31/ ((PI()*4^2*40)*0.0014*0.3*(1/0.917)*10)</f>
-        <v>2171.80182760816</v>
+        <f aca="false">1E-034*L31*EXP(87.015*L31)</f>
+        <v>5091.31557007718</v>
       </c>
       <c r="N31" s="0" t="n">
-        <v>0.997820679177718</v>
-      </c>
-      <c r="O31" s="0" t="n">
-        <f aca="false">1E-034*N31*EXP(87.015*N31)</f>
-        <v>5091.31557007718</v>
-      </c>
-      <c r="P31" s="0" t="n">
-        <f aca="false">ABS(M31-I31)</f>
+        <f aca="false">ABS(K31-I31)</f>
         <v>1233.80182760816</v>
       </c>
+      <c r="S31" s="2"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>1200</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>24</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E32" s="1"/>
       <c r="F32" s="0" t="n">
         <v>400</v>
       </c>
@@ -1968,43 +1827,39 @@
         <v>13438</v>
       </c>
       <c r="J32" s="0" t="n">
-        <v>0.4</v>
+        <v>99441.2</v>
       </c>
       <c r="K32" s="0" t="n">
-        <v>4972.06</v>
+        <f aca="false">H32/ (      (((((PI()*4^2)*40)*0.0014)*0.3)/0.917)*10   )</f>
+        <v>21718.0182760816</v>
       </c>
       <c r="L32" s="0" t="n">
-        <v>99441.2</v>
+        <v>0.998519805358618</v>
       </c>
       <c r="M32" s="0" t="n">
-        <f aca="false">H32/ ((PI()*4^2*40)*0.0014*0.3*(1/0.917)*10)</f>
-        <v>21718.0182760816</v>
+        <f aca="false">1E-034*L32*EXP(87.015*L32)</f>
+        <v>5414.44905630543</v>
       </c>
       <c r="N32" s="0" t="n">
-        <v>0.998519805358618</v>
-      </c>
-      <c r="O32" s="0" t="n">
-        <f aca="false">1E-034*N32*EXP(87.015*N32)</f>
-        <v>5414.4490563052</v>
-      </c>
-      <c r="P32" s="0" t="n">
-        <f aca="false">ABS(M32-I32)</f>
+        <f aca="false">ABS(K32-I32)</f>
         <v>8280.01827608155</v>
       </c>
+      <c r="S32" s="2"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>1142</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>21</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="E33" s="1"/>
       <c r="F33" s="0" t="n">
         <v>700</v>
       </c>
@@ -2018,50 +1873,45 @@
         <v>750</v>
       </c>
       <c r="J33" s="0" t="n">
-        <v>0.7</v>
+        <v>5550</v>
       </c>
       <c r="K33" s="0" t="n">
-        <v>277.5</v>
+        <f aca="false">H33/ (      (((((PI()*4^2)*40)*0.0014)*0.3)/0.917)*10   )</f>
+        <v>2171.80182760816</v>
       </c>
       <c r="L33" s="0" t="n">
-        <v>5550</v>
+        <v>0.999178426545775</v>
       </c>
       <c r="M33" s="0" t="n">
-        <f aca="false">H33/ ((PI()*4^2*40)*0.0014*0.3*(1/0.917)*10)</f>
-        <v>2171.80182760816</v>
+        <f aca="false">1E-034*L33*EXP(87.015*L33)</f>
+        <v>5737.59672693878</v>
       </c>
       <c r="N33" s="0" t="n">
-        <v>0.999178426545775</v>
-      </c>
-      <c r="O33" s="0" t="n">
-        <f aca="false">1E-034*N33*EXP(87.015*N33)</f>
-        <v>5737.59672693862</v>
-      </c>
-      <c r="P33" s="0" t="n">
-        <f aca="false">ABS(M33-I33)</f>
+        <f aca="false">ABS(K33-I33)</f>
         <v>1421.80182760816</v>
       </c>
+      <c r="S33" s="2"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H34" s="2"/>
-      <c r="L34" s="2"/>
-      <c r="N34" s="2"/>
+      <c r="H34" s="4"/>
+      <c r="L34" s="4"/>
+      <c r="N34" s="4"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O35" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="P35" s="0" t="n">
-        <f aca="false">AVERAGE(P2:P33)</f>
+      <c r="M35" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="N35" s="0" t="n">
+        <f aca="false">AVERAGE(N2:N33)</f>
         <v>6592.55229549229</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O36" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="P36" s="0" t="n">
-        <f aca="false">STDEV(P2:P33)</f>
+      <c r="M36" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="N36" s="0" t="n">
+        <f aca="false">STDEV(N2:N33)</f>
         <v>7539.98932160151</v>
       </c>
     </row>

</xml_diff>